<commit_message>
Elimina duplicados en el archivo de Anulados y ajusta la preparación de columnas finales en la integración de Pacífico
</commit_message>
<xml_diff>
--- a/src/app/data/input/PreparaciónPacífico/Anulados/Anulados.xlsx
+++ b/src/app/data/input/PreparaciónPacífico/Anulados/Anulados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renzo Araujo\PycharmProjects\GestorDeValidaciones\src\app\data\input\PreparaciónPacífico\Anulados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE0A539-80F2-4143-AC8F-174606D8F320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8111AA69-CFBD-42EB-ABFD-B99B6F8E8122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -962,11 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H339"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1053,7 +1052,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -1153,7 +1152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
@@ -1175,7 +1174,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -1201,7 +1200,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
@@ -1227,7 +1226,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
@@ -1275,7 +1274,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -1323,7 +1322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -1375,7 +1374,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -1401,7 +1400,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
@@ -1423,7 +1422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>33</v>
       </c>
@@ -1471,7 +1470,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>34</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>37</v>
       </c>
@@ -1541,7 +1540,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>40</v>
       </c>
@@ -1567,7 +1566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>40</v>
       </c>
@@ -1593,7 +1592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>41</v>
       </c>
@@ -1619,7 +1618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>42</v>
       </c>
@@ -1641,7 +1640,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>43</v>
       </c>
@@ -1663,7 +1662,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>44</v>
       </c>
@@ -1685,7 +1684,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>45</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>45</v>
       </c>
@@ -1755,7 +1754,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>47</v>
       </c>
@@ -1803,7 +1802,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>8</v>
       </c>
@@ -1903,7 +1902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>54</v>
       </c>
@@ -1955,7 +1954,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>58</v>
       </c>
@@ -1981,7 +1980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>58</v>
       </c>
@@ -2007,7 +2006,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>59</v>
       </c>
@@ -2055,7 +2054,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>62</v>
       </c>
@@ -2081,7 +2080,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>63</v>
       </c>
@@ -2107,7 +2106,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>63</v>
       </c>
@@ -2129,7 +2128,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>63</v>
       </c>
@@ -2155,7 +2154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>63</v>
       </c>
@@ -2181,7 +2180,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>64</v>
       </c>
@@ -2203,7 +2202,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>65</v>
       </c>
@@ -2225,7 +2224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>66</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>66</v>
       </c>
@@ -2329,7 +2328,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>70</v>
       </c>
@@ -2433,7 +2432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>70</v>
       </c>
@@ -2479,7 +2478,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>70</v>
       </c>
@@ -2501,7 +2500,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>70</v>
       </c>
@@ -2527,7 +2526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>70</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>73</v>
       </c>
@@ -2601,7 +2600,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>74</v>
       </c>
@@ -2627,7 +2626,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>74</v>
       </c>
@@ -2705,7 +2704,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>76</v>
       </c>
@@ -2783,7 +2782,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>78</v>
       </c>
@@ -2809,7 +2808,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>79</v>
       </c>
@@ -2857,7 +2856,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>81</v>
       </c>
@@ -2879,7 +2878,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>82</v>
       </c>
@@ -2901,7 +2900,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>84</v>
       </c>
@@ -2953,7 +2952,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>84</v>
       </c>
@@ -2975,7 +2974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>85</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>87</v>
       </c>
@@ -3131,7 +3130,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>87</v>
       </c>
@@ -3177,7 +3176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>87</v>
       </c>
@@ -3199,7 +3198,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>87</v>
       </c>
@@ -3225,7 +3224,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>87</v>
       </c>
@@ -3251,7 +3250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>31</v>
       </c>
@@ -3277,7 +3276,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>88</v>
       </c>
@@ -3303,7 +3302,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>89</v>
       </c>
@@ -3355,7 +3354,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>89</v>
       </c>
@@ -3401,7 +3400,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>89</v>
       </c>
@@ -3423,7 +3422,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>90</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>90</v>
       </c>
@@ -3497,7 +3496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>90</v>
       </c>
@@ -3545,7 +3544,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>92</v>
       </c>
@@ -3567,7 +3566,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>93</v>
       </c>
@@ -3593,7 +3592,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>93</v>
       </c>
@@ -3619,7 +3618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>95</v>
       </c>
@@ -3723,7 +3722,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>95</v>
       </c>
@@ -3749,7 +3748,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>95</v>
       </c>
@@ -3827,7 +3826,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>99</v>
       </c>
@@ -3849,7 +3848,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>97</v>
       </c>
@@ -3875,7 +3874,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>99</v>
       </c>
@@ -3951,7 +3950,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>61</v>
       </c>
@@ -3997,7 +3996,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>61</v>
       </c>
@@ -4019,7 +4018,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>37</v>
       </c>
@@ -4041,7 +4040,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>93</v>
       </c>
@@ -4063,7 +4062,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>103</v>
       </c>
@@ -4085,7 +4084,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>103</v>
       </c>
@@ -4107,7 +4106,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>104</v>
       </c>
@@ -4129,7 +4128,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>104</v>
       </c>
@@ -4151,7 +4150,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>106</v>
       </c>
@@ -4173,7 +4172,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>106</v>
       </c>
@@ -4195,7 +4194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>108</v>
       </c>
@@ -4269,7 +4268,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>111</v>
       </c>
@@ -4397,7 +4396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>111</v>
       </c>
@@ -4423,7 +4422,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>111</v>
       </c>
@@ -4449,7 +4448,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>115</v>
       </c>
@@ -4553,7 +4552,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>115</v>
       </c>
@@ -4579,7 +4578,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>115</v>
       </c>
@@ -4629,7 +4628,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>108</v>
       </c>
@@ -4651,7 +4650,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>54</v>
       </c>
@@ -4729,7 +4728,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>54</v>
       </c>
@@ -4751,7 +4750,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>54</v>
       </c>
@@ -4777,7 +4776,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>54</v>
       </c>
@@ -4829,7 +4828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
         <v>47</v>
       </c>
@@ -4851,7 +4850,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>47</v>
       </c>
@@ -4873,7 +4872,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
         <v>119</v>
       </c>
@@ -4895,7 +4894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
         <v>120</v>
       </c>
@@ -4917,7 +4916,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
         <v>120</v>
       </c>
@@ -4965,7 +4964,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
         <v>121</v>
       </c>
@@ -5011,7 +5010,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
         <v>121</v>
       </c>
@@ -5059,7 +5058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
         <v>124</v>
       </c>
@@ -5105,7 +5104,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
         <v>124</v>
       </c>
@@ -5153,7 +5152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
         <v>15</v>
       </c>
@@ -5257,7 +5256,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
         <v>128</v>
       </c>
@@ -5303,7 +5302,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
         <v>125</v>
       </c>
@@ -5325,7 +5324,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
         <v>15</v>
       </c>
@@ -5351,7 +5350,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
         <v>129</v>
       </c>
@@ -5377,7 +5376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
         <v>20</v>
       </c>
@@ -5399,7 +5398,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
         <v>45</v>
       </c>
@@ -5425,7 +5424,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
         <v>45</v>
       </c>
@@ -5447,7 +5446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="6" t="s">
         <v>45</v>
       </c>
@@ -5495,7 +5494,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="6" t="s">
         <v>47</v>
       </c>
@@ -5517,7 +5516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
         <v>47</v>
       </c>
@@ -5565,7 +5564,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
         <v>8</v>
       </c>
@@ -5587,7 +5586,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="6" t="s">
         <v>8</v>
       </c>
@@ -5713,7 +5712,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
         <v>59</v>
       </c>
@@ -5735,7 +5734,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="6" t="s">
         <v>58</v>
       </c>
@@ -5761,7 +5760,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="6" t="s">
         <v>63</v>
       </c>
@@ -5839,7 +5838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
         <v>63</v>
       </c>
@@ -5861,7 +5860,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="6" t="s">
         <v>63</v>
       </c>
@@ -5887,7 +5886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="6" t="s">
         <v>63</v>
       </c>
@@ -5913,7 +5912,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="6" t="s">
         <v>66</v>
       </c>
@@ -5991,7 +5990,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="6" t="s">
         <v>66</v>
       </c>
@@ -6013,7 +6012,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="6" t="s">
         <v>66</v>
       </c>
@@ -6039,7 +6038,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="6" t="s">
         <v>66</v>
       </c>
@@ -6091,7 +6090,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="6" t="s">
         <v>131</v>
       </c>
@@ -6117,7 +6116,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
         <v>131</v>
       </c>
@@ -6139,7 +6138,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
         <v>73</v>
       </c>
@@ -6213,7 +6212,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="13" t="s">
         <v>132</v>
       </c>
@@ -6239,7 +6238,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="6" t="s">
         <v>84</v>
       </c>
@@ -6343,7 +6342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
         <v>84</v>
       </c>
@@ -6365,7 +6364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
         <v>84</v>
       </c>
@@ -6417,7 +6416,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="222" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
         <v>133</v>
       </c>
@@ -6495,7 +6494,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
         <v>133</v>
       </c>
@@ -6517,7 +6516,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
         <v>133</v>
       </c>
@@ -6539,7 +6538,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
         <v>133</v>
       </c>
@@ -6565,7 +6564,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
         <v>133</v>
       </c>
@@ -6617,7 +6616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="6" t="s">
         <v>87</v>
       </c>
@@ -6721,7 +6720,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
         <v>87</v>
       </c>
@@ -6767,7 +6766,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="6" t="s">
         <v>87</v>
       </c>
@@ -6789,7 +6788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="6" t="s">
         <v>87</v>
       </c>
@@ -6815,7 +6814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
         <v>87</v>
       </c>
@@ -6841,7 +6840,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="6" t="s">
         <v>31</v>
       </c>
@@ -6867,7 +6866,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="13" t="s">
         <v>85</v>
       </c>
@@ -6893,7 +6892,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="6" t="s">
         <v>90</v>
       </c>
@@ -6945,7 +6944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="6" t="s">
         <v>90</v>
       </c>
@@ -6967,7 +6966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="6" t="s">
         <v>90</v>
       </c>
@@ -7015,7 +7014,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="13" t="s">
         <v>92</v>
       </c>
@@ -7037,7 +7036,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="13" t="s">
         <v>95</v>
       </c>
@@ -7059,7 +7058,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="6" t="s">
         <v>95</v>
       </c>
@@ -7081,7 +7080,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="6" t="s">
         <v>95</v>
       </c>
@@ -7107,7 +7106,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="6" t="s">
         <v>95</v>
       </c>
@@ -7133,7 +7132,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="6" t="s">
         <v>139</v>
       </c>
@@ -7159,7 +7158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="6" t="s">
         <v>139</v>
       </c>
@@ -7233,7 +7232,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="6" t="s">
         <v>99</v>
       </c>
@@ -7255,7 +7254,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="6" t="s">
         <v>97</v>
       </c>
@@ -7281,7 +7280,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="6" t="s">
         <v>99</v>
       </c>
@@ -7357,7 +7356,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="6" t="s">
         <v>61</v>
       </c>
@@ -7403,7 +7402,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="6" t="s">
         <v>61</v>
       </c>
@@ -7425,7 +7424,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="6" t="s">
         <v>37</v>
       </c>
@@ -7447,7 +7446,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="6" t="s">
         <v>93</v>
       </c>
@@ -7469,7 +7468,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="6" t="s">
         <v>103</v>
       </c>
@@ -7491,7 +7490,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" s="6" t="s">
         <v>103</v>
       </c>
@@ -7513,7 +7512,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="6" t="s">
         <v>104</v>
       </c>
@@ -7535,7 +7534,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="6" t="s">
         <v>104</v>
       </c>
@@ -7557,7 +7556,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="6" t="s">
         <v>140</v>
       </c>
@@ -7579,7 +7578,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" s="6" t="s">
         <v>140</v>
       </c>
@@ -7601,7 +7600,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="6" t="s">
         <v>106</v>
       </c>
@@ -7623,7 +7622,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="6" t="s">
         <v>106</v>
       </c>
@@ -7645,7 +7644,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="6" t="s">
         <v>141</v>
       </c>
@@ -7667,7 +7666,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="6" t="s">
         <v>8</v>
       </c>
@@ -7689,7 +7688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="6" t="s">
         <v>34</v>
       </c>
@@ -7711,7 +7710,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="6" t="s">
         <v>47</v>
       </c>
@@ -7733,7 +7732,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="6" t="s">
         <v>8</v>
       </c>
@@ -7755,7 +7754,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="6" t="s">
         <v>82</v>
       </c>
@@ -7777,7 +7776,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="6" t="s">
         <v>92</v>
       </c>
@@ -7799,7 +7798,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
         <v>99</v>
       </c>
@@ -7821,7 +7820,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="6" t="s">
         <v>104</v>
       </c>
@@ -7843,7 +7842,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
         <v>47</v>
       </c>
@@ -7865,7 +7864,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
         <v>47</v>
       </c>
@@ -7887,7 +7886,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
         <v>8</v>
       </c>
@@ -7909,7 +7908,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285" s="6" t="s">
         <v>133</v>
       </c>
@@ -7931,7 +7930,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286" s="6" t="s">
         <v>92</v>
       </c>
@@ -7953,7 +7952,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287" s="6" t="s">
         <v>95</v>
       </c>
@@ -7975,7 +7974,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288" s="6" t="s">
         <v>99</v>
       </c>
@@ -7997,7 +7996,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289" s="6" t="s">
         <v>104</v>
       </c>
@@ -8019,7 +8018,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" s="6" t="s">
         <v>140</v>
       </c>
@@ -8041,7 +8040,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291" s="6" t="s">
         <v>121</v>
       </c>
@@ -8063,7 +8062,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292" s="6" t="s">
         <v>124</v>
       </c>
@@ -8085,7 +8084,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293" s="6" t="s">
         <v>20</v>
       </c>
@@ -8107,7 +8106,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294" s="6" t="s">
         <v>23</v>
       </c>
@@ -8129,7 +8128,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295" s="6" t="s">
         <v>20</v>
       </c>
@@ -8151,7 +8150,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296" s="6" t="s">
         <v>28</v>
       </c>
@@ -8173,7 +8172,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297" s="6" t="s">
         <v>33</v>
       </c>
@@ -8195,7 +8194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298" s="6" t="s">
         <v>37</v>
       </c>
@@ -8217,7 +8216,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299" s="6" t="s">
         <v>42</v>
       </c>
@@ -8239,7 +8238,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
         <v>43</v>
       </c>
@@ -8261,7 +8260,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301" s="6" t="s">
         <v>44</v>
       </c>
@@ -8283,7 +8282,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302" s="6" t="s">
         <v>45</v>
       </c>
@@ -8305,7 +8304,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303" s="6" t="s">
         <v>63</v>
       </c>
@@ -8327,7 +8326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304" s="6" t="s">
         <v>64</v>
       </c>
@@ -8349,7 +8348,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305" s="6" t="s">
         <v>65</v>
       </c>
@@ -8371,7 +8370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306" s="6" t="s">
         <v>70</v>
       </c>
@@ -8393,7 +8392,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" s="6" t="s">
         <v>73</v>
       </c>
@@ -8415,7 +8414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308" s="6" t="s">
         <v>79</v>
       </c>
@@ -8437,7 +8436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309" s="6" t="s">
         <v>81</v>
       </c>
@@ -8459,7 +8458,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="310" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310" s="6" t="s">
         <v>84</v>
       </c>
@@ -8481,7 +8480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311" s="6" t="s">
         <v>87</v>
       </c>
@@ -8503,7 +8502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312" s="6" t="s">
         <v>89</v>
       </c>
@@ -8525,7 +8524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313" s="6" t="s">
         <v>90</v>
       </c>
@@ -8547,7 +8546,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314" s="6" t="s">
         <v>61</v>
       </c>
@@ -8569,7 +8568,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315" s="6" t="s">
         <v>37</v>
       </c>
@@ -8591,7 +8590,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316" s="6" t="s">
         <v>93</v>
       </c>
@@ -8613,7 +8612,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317" s="6" t="s">
         <v>103</v>
       </c>
@@ -8635,7 +8634,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318" s="6" t="s">
         <v>106</v>
       </c>
@@ -8657,7 +8656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="319" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319" s="6" t="s">
         <v>108</v>
       </c>
@@ -8679,7 +8678,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320" s="6" t="s">
         <v>108</v>
       </c>
@@ -8701,7 +8700,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321" s="6" t="s">
         <v>54</v>
       </c>
@@ -8723,7 +8722,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322" s="6" t="s">
         <v>120</v>
       </c>
@@ -8745,7 +8744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323" s="6" t="s">
         <v>120</v>
       </c>
@@ -8767,7 +8766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324" s="6" t="s">
         <v>125</v>
       </c>
@@ -8789,7 +8788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325" s="6" t="s">
         <v>20</v>
       </c>
@@ -8811,7 +8810,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326" s="6" t="s">
         <v>45</v>
       </c>
@@ -8833,7 +8832,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327" s="6" t="s">
         <v>63</v>
       </c>
@@ -8855,7 +8854,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328" s="6" t="s">
         <v>66</v>
       </c>
@@ -8877,7 +8876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329" s="6" t="s">
         <v>131</v>
       </c>
@@ -8899,7 +8898,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330" s="6" t="s">
         <v>73</v>
       </c>
@@ -8921,7 +8920,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331" s="6" t="s">
         <v>84</v>
       </c>
@@ -8943,7 +8942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332" s="6" t="s">
         <v>87</v>
       </c>
@@ -8965,7 +8964,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333" s="6" t="s">
         <v>90</v>
       </c>
@@ -8987,7 +8986,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334" s="6" t="s">
         <v>139</v>
       </c>
@@ -9009,7 +9008,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335" s="6" t="s">
         <v>61</v>
       </c>
@@ -9031,7 +9030,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336" s="6" t="s">
         <v>37</v>
       </c>
@@ -9053,7 +9052,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" s="6" t="s">
         <v>93</v>
       </c>
@@ -9075,7 +9074,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" s="6" t="s">
         <v>103</v>
       </c>
@@ -9097,7 +9096,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" s="6" t="s">
         <v>106</v>
       </c>
@@ -9120,14 +9119,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H339" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <dateGroupItem year="2026" dateTimeGrouping="year"/>
-        <dateGroupItem year="2025" dateTimeGrouping="year"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H339" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="D1:D339">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>